<commit_message>
geracao ok. Mas falta zipar pro sala e nao por candidato
</commit_message>
<xml_diff>
--- a/src/inscritos_aceitos(1).xlsx
+++ b/src/inscritos_aceitos(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\gerador-de-prova-escrita\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487BEBED-A785-46EF-8E9D-19E09A8A4C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB057196-5BC0-49D8-8B6A-FC0C6D1C982B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2355" yWindow="2040" windowWidth="32190" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="593">
   <si>
     <t>NOME</t>
   </si>
@@ -1370,6 +1370,435 @@
   </si>
   <si>
     <t>INSCRIÇÃO</t>
+  </si>
+  <si>
+    <t>389447-Amapá</t>
+  </si>
+  <si>
+    <t>165808-Ssp/ap</t>
+  </si>
+  <si>
+    <t>094524-Amapá</t>
+  </si>
+  <si>
+    <t>080062-Amapá</t>
+  </si>
+  <si>
+    <t>143983-Ap</t>
+  </si>
+  <si>
+    <t>256017-Ssap</t>
+  </si>
+  <si>
+    <t>7210826-Pará</t>
+  </si>
+  <si>
+    <t>401687-Politec</t>
+  </si>
+  <si>
+    <t>143876-Ap</t>
+  </si>
+  <si>
+    <t>487237-Amapá</t>
+  </si>
+  <si>
+    <t>529369-Politec</t>
+  </si>
+  <si>
+    <t>332015-Ap</t>
+  </si>
+  <si>
+    <t>481915-Amapá</t>
+  </si>
+  <si>
+    <t>385779-Ap</t>
+  </si>
+  <si>
+    <t>613689-Amapá</t>
+  </si>
+  <si>
+    <t>187983-Amapá</t>
+  </si>
+  <si>
+    <t>732139-Amapá</t>
+  </si>
+  <si>
+    <t>646021-Ap</t>
+  </si>
+  <si>
+    <t>504119-Ap</t>
+  </si>
+  <si>
+    <t>331710-Ap</t>
+  </si>
+  <si>
+    <t>376253-Ap</t>
+  </si>
+  <si>
+    <t>469015-Amapá</t>
+  </si>
+  <si>
+    <t>391493-Ssp</t>
+  </si>
+  <si>
+    <t>164816-Amapá</t>
+  </si>
+  <si>
+    <t>669892-Amapá</t>
+  </si>
+  <si>
+    <t>586278-Ap</t>
+  </si>
+  <si>
+    <t>673625-Amapá</t>
+  </si>
+  <si>
+    <t>147286-Ap</t>
+  </si>
+  <si>
+    <t>442179-Ap</t>
+  </si>
+  <si>
+    <t>449442-Amapá</t>
+  </si>
+  <si>
+    <t>625752-Siac</t>
+  </si>
+  <si>
+    <t>470862-Amapá (Ap)</t>
+  </si>
+  <si>
+    <t>610531-Amapá</t>
+  </si>
+  <si>
+    <t>550792-Macapá</t>
+  </si>
+  <si>
+    <t>505138-Amapá</t>
+  </si>
+  <si>
+    <t>146434-Ap</t>
+  </si>
+  <si>
+    <t>413039-Ap</t>
+  </si>
+  <si>
+    <t>491458-Amapá</t>
+  </si>
+  <si>
+    <t>409252-Ap</t>
+  </si>
+  <si>
+    <t>1717-50-Amapa</t>
+  </si>
+  <si>
+    <t>701003-Amapá</t>
+  </si>
+  <si>
+    <t>483595-Amapá</t>
+  </si>
+  <si>
+    <t>476827-Amapá</t>
+  </si>
+  <si>
+    <t>352543-Amapá</t>
+  </si>
+  <si>
+    <t>085302-Amapá</t>
+  </si>
+  <si>
+    <t>667845537-São Paulo</t>
+  </si>
+  <si>
+    <t>425079-Amapa</t>
+  </si>
+  <si>
+    <t>293946-Amapá</t>
+  </si>
+  <si>
+    <t>387936-Politec</t>
+  </si>
+  <si>
+    <t>157822-Ap</t>
+  </si>
+  <si>
+    <t>533558-Amapá</t>
+  </si>
+  <si>
+    <t>553908-Ap</t>
+  </si>
+  <si>
+    <t>173339-Ap</t>
+  </si>
+  <si>
+    <t>580485-Amapá</t>
+  </si>
+  <si>
+    <t>551400-Ap</t>
+  </si>
+  <si>
+    <t>586482-Amapaense</t>
+  </si>
+  <si>
+    <t>554951-Ap</t>
+  </si>
+  <si>
+    <t>123873-Ap</t>
+  </si>
+  <si>
+    <t>198142-Amapá</t>
+  </si>
+  <si>
+    <t>528435-Ap</t>
+  </si>
+  <si>
+    <t>7322152-Pará</t>
+  </si>
+  <si>
+    <t>642338-Ap</t>
+  </si>
+  <si>
+    <t>667380-Amapá</t>
+  </si>
+  <si>
+    <t>135545-Ap</t>
+  </si>
+  <si>
+    <t>594437-Amapá</t>
+  </si>
+  <si>
+    <t>335471-Amapá</t>
+  </si>
+  <si>
+    <t>524163-Amapá</t>
+  </si>
+  <si>
+    <t>452028-Amapá</t>
+  </si>
+  <si>
+    <t>460662-Ap</t>
+  </si>
+  <si>
+    <t>554636-Siac</t>
+  </si>
+  <si>
+    <t>296370-Amapá</t>
+  </si>
+  <si>
+    <t>368815-Politec</t>
+  </si>
+  <si>
+    <t>417036-Amapá</t>
+  </si>
+  <si>
+    <t>6272243-Policia Civil</t>
+  </si>
+  <si>
+    <t>647586-Ap</t>
+  </si>
+  <si>
+    <t>195374-Ap</t>
+  </si>
+  <si>
+    <t>431657-Ap</t>
+  </si>
+  <si>
+    <t>549525-Ap</t>
+  </si>
+  <si>
+    <t>857257-Politec</t>
+  </si>
+  <si>
+    <t>900950-Solteira</t>
+  </si>
+  <si>
+    <t>174930-Siac</t>
+  </si>
+  <si>
+    <t>515252-Ap</t>
+  </si>
+  <si>
+    <t>847010-Ptcdicc</t>
+  </si>
+  <si>
+    <t>447448-Ap</t>
+  </si>
+  <si>
+    <t>422461-Ap</t>
+  </si>
+  <si>
+    <t>621546-Politec</t>
+  </si>
+  <si>
+    <t>385407-Ap</t>
+  </si>
+  <si>
+    <t>226048-Ap</t>
+  </si>
+  <si>
+    <t>473664-Amapá</t>
+  </si>
+  <si>
+    <t>577490-Amapá</t>
+  </si>
+  <si>
+    <t>374203-Ap</t>
+  </si>
+  <si>
+    <t>573416-Ap</t>
+  </si>
+  <si>
+    <t>103905-Amapá</t>
+  </si>
+  <si>
+    <t>555691-Amapá</t>
+  </si>
+  <si>
+    <t>6243910-Pa</t>
+  </si>
+  <si>
+    <t>522938-Amapá</t>
+  </si>
+  <si>
+    <t>440227-Ap</t>
+  </si>
+  <si>
+    <t>509370-Amapá</t>
+  </si>
+  <si>
+    <t>593804-Amapá</t>
+  </si>
+  <si>
+    <t>411401-Ap</t>
+  </si>
+  <si>
+    <t>524014-Siac</t>
+  </si>
+  <si>
+    <t>356207-Ap</t>
+  </si>
+  <si>
+    <t>341370-Ap</t>
+  </si>
+  <si>
+    <t>647940-Amapá</t>
+  </si>
+  <si>
+    <t>164011-Ap</t>
+  </si>
+  <si>
+    <t>520746-Ap</t>
+  </si>
+  <si>
+    <t>156379-Amapá</t>
+  </si>
+  <si>
+    <t>5081029-Segup/pa</t>
+  </si>
+  <si>
+    <t>505162-Ap</t>
+  </si>
+  <si>
+    <t>457881-Amapá</t>
+  </si>
+  <si>
+    <t>358821-Amapá</t>
+  </si>
+  <si>
+    <t>256016-Ssap</t>
+  </si>
+  <si>
+    <t>559209-Politec</t>
+  </si>
+  <si>
+    <t>672843-Amapá - Ap</t>
+  </si>
+  <si>
+    <t>599345-Ap</t>
+  </si>
+  <si>
+    <t>598818-Amapá</t>
+  </si>
+  <si>
+    <t>904570-Politec</t>
+  </si>
+  <si>
+    <t>594422-Amapá</t>
+  </si>
+  <si>
+    <t>612823-Amapá</t>
+  </si>
+  <si>
+    <t>467340-Ap</t>
+  </si>
+  <si>
+    <t>688628-Amapá</t>
+  </si>
+  <si>
+    <t>7107347-Pa</t>
+  </si>
+  <si>
+    <t>650232-Amapá</t>
+  </si>
+  <si>
+    <t>425087-Ap</t>
+  </si>
+  <si>
+    <t>555952-Ap</t>
+  </si>
+  <si>
+    <t>256472-Ap</t>
+  </si>
+  <si>
+    <t>469693-Ap</t>
+  </si>
+  <si>
+    <t>549526-Amapá</t>
+  </si>
+  <si>
+    <t>337750-Ap</t>
+  </si>
+  <si>
+    <t>510487-Ap</t>
+  </si>
+  <si>
+    <t>366180-Amapá</t>
+  </si>
+  <si>
+    <t>569357-Ap</t>
+  </si>
+  <si>
+    <t>280699-Amapá</t>
+  </si>
+  <si>
+    <t>131884-Amapá</t>
+  </si>
+  <si>
+    <t>471864-Dptc</t>
+  </si>
+  <si>
+    <t>564176-Amapá</t>
+  </si>
+  <si>
+    <t>106179-Amapá</t>
+  </si>
+  <si>
+    <t>15806860-5-Ssp/pr</t>
+  </si>
+  <si>
+    <t>0738416620218-Maranhão</t>
+  </si>
+  <si>
+    <t>340573-Ap</t>
+  </si>
+  <si>
+    <t>328870-Amapá</t>
+  </si>
+  <si>
+    <t>7902213-Policia Civil</t>
+  </si>
+  <si>
+    <t>RG</t>
   </si>
 </sst>
 </file>
@@ -1711,10 +2140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:G143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1724,10 +2153,12 @@
     <col min="3" max="3" width="57.28515625" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1746,8 +2177,11 @@
       <c r="F1" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1760,8 +2194,11 @@
       <c r="F2" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1780,8 +2217,11 @@
       <c r="F3" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1800,8 +2240,11 @@
       <c r="F4" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1820,8 +2263,11 @@
       <c r="F5" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1840,8 +2286,11 @@
       <c r="F6" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1860,8 +2309,11 @@
       <c r="F7" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1880,8 +2332,11 @@
       <c r="F8" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1900,8 +2355,11 @@
       <c r="F9" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1920,8 +2378,11 @@
       <c r="F10" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1940,8 +2401,11 @@
       <c r="F11" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1960,8 +2424,11 @@
       <c r="F12" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1980,8 +2447,11 @@
       <c r="F13" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2000,8 +2470,11 @@
       <c r="F14" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2020,8 +2493,11 @@
       <c r="F15" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2040,8 +2516,11 @@
       <c r="F16" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2060,8 +2539,11 @@
       <c r="F17" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2080,8 +2562,11 @@
       <c r="F18" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2100,8 +2585,11 @@
       <c r="F19" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2120,8 +2608,11 @@
       <c r="F20" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G20" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2140,8 +2631,11 @@
       <c r="F21" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G21" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2160,8 +2654,11 @@
       <c r="F22" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G22" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2180,8 +2677,11 @@
       <c r="F23" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G23" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -2200,8 +2700,11 @@
       <c r="F24" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G24" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2220,8 +2723,11 @@
       <c r="F25" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G25" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2240,8 +2746,11 @@
       <c r="F26" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G26" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2260,8 +2769,11 @@
       <c r="F27" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G27" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -2280,8 +2792,11 @@
       <c r="F28" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G28" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -2300,8 +2815,11 @@
       <c r="F29" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G29" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2320,8 +2838,11 @@
       <c r="F30" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G30" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -2340,8 +2861,11 @@
       <c r="F31" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G31" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2360,8 +2884,11 @@
       <c r="F32" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G32" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -2380,8 +2907,11 @@
       <c r="F33" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G33" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -2400,8 +2930,11 @@
       <c r="F34" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G34" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2420,8 +2953,11 @@
       <c r="F35" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G35" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2440,8 +2976,11 @@
       <c r="F36" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G36" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2460,8 +2999,11 @@
       <c r="F37" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G37" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2480,8 +3022,11 @@
       <c r="F38" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G38" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -2500,8 +3045,11 @@
       <c r="F39" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G39" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2520,8 +3068,11 @@
       <c r="F40" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G40" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2540,8 +3091,11 @@
       <c r="F41" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G41" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2560,8 +3114,11 @@
       <c r="F42" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G42" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2580,8 +3137,11 @@
       <c r="F43" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G43" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2600,8 +3160,11 @@
       <c r="F44" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G44" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2620,8 +3183,11 @@
       <c r="F45" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G45" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2640,8 +3206,11 @@
       <c r="F46" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G46" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2660,8 +3229,11 @@
       <c r="F47" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G47" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2680,8 +3252,11 @@
       <c r="F48" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G48" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2700,8 +3275,11 @@
       <c r="F49" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G49" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2720,8 +3298,11 @@
       <c r="F50" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G50" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -2740,8 +3321,11 @@
       <c r="F51" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G51" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -2760,8 +3344,11 @@
       <c r="F52" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G52" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -2780,8 +3367,11 @@
       <c r="F53" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G53" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -2800,8 +3390,11 @@
       <c r="F54" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G54" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -2820,8 +3413,11 @@
       <c r="F55" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G55" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -2840,8 +3436,11 @@
       <c r="F56" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G56" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -2860,8 +3459,11 @@
       <c r="F57" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G57" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -2880,8 +3482,11 @@
       <c r="F58" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G58" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -2900,8 +3505,11 @@
       <c r="F59" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G59" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -2920,8 +3528,11 @@
       <c r="F60" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G60" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -2940,8 +3551,11 @@
       <c r="F61" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G61" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -2960,8 +3574,11 @@
       <c r="F62" s="1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G62" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" customHeight="1">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -2980,8 +3597,11 @@
       <c r="F63" s="1" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G63" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" customHeight="1">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -3000,8 +3620,11 @@
       <c r="F64" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G64" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" customHeight="1">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -3020,8 +3643,11 @@
       <c r="F65" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G65" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -3040,8 +3666,11 @@
       <c r="F66" s="1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G66" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15.75" customHeight="1">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -3060,8 +3689,11 @@
       <c r="F67" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G67" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" customHeight="1">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -3080,8 +3712,11 @@
       <c r="F68" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G68" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" customHeight="1">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -3100,8 +3735,11 @@
       <c r="F69" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G69" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.75" customHeight="1">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -3120,8 +3758,11 @@
       <c r="F70" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G70" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" customHeight="1">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -3140,8 +3781,11 @@
       <c r="F71" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G71" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" customHeight="1">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -3160,8 +3804,11 @@
       <c r="F72" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G72" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.75" customHeight="1">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -3180,8 +3827,11 @@
       <c r="F73" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G73" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.75" customHeight="1">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -3200,8 +3850,11 @@
       <c r="F74" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G74" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15.75" customHeight="1">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -3220,8 +3873,11 @@
       <c r="F75" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G75" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="15.75" customHeight="1">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -3240,8 +3896,11 @@
       <c r="F76" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G76" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15.75" customHeight="1">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -3260,8 +3919,11 @@
       <c r="F77" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G77" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15.75" customHeight="1">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -3280,8 +3942,11 @@
       <c r="F78" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G78" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15.75" customHeight="1">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -3300,8 +3965,11 @@
       <c r="F79" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G79" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15.75" customHeight="1">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -3320,8 +3988,11 @@
       <c r="F80" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G80" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15.75" customHeight="1">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -3340,8 +4011,11 @@
       <c r="F81" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G81" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15.75" customHeight="1">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -3360,8 +4034,11 @@
       <c r="F82" s="1" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G82" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15.75" customHeight="1">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -3380,8 +4057,11 @@
       <c r="F83" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G83" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15.75" customHeight="1">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -3400,8 +4080,11 @@
       <c r="F84" s="1" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G84" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" customHeight="1">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -3420,8 +4103,11 @@
       <c r="F85" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G85" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15.75" customHeight="1">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -3440,8 +4126,11 @@
       <c r="F86" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G86" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" customHeight="1">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -3460,8 +4149,11 @@
       <c r="F87" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G87" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" customHeight="1">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -3480,8 +4172,11 @@
       <c r="F88" s="1" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G88" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15.75" customHeight="1">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -3500,8 +4195,11 @@
       <c r="F89" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G89" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="15.75" customHeight="1">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -3520,8 +4218,11 @@
       <c r="F90" s="1" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G90" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="15.75" customHeight="1">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -3540,8 +4241,11 @@
       <c r="F91" s="1" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G91" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="15.75" customHeight="1">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -3560,8 +4264,11 @@
       <c r="F92" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G92" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="15.75" customHeight="1">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -3580,8 +4287,11 @@
       <c r="F93" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G93" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="15.75" customHeight="1">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -3600,8 +4310,11 @@
       <c r="F94" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G94" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15.75" customHeight="1">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -3620,8 +4333,11 @@
       <c r="F95" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G95" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15.75" customHeight="1">
       <c r="A96" t="s">
         <v>104</v>
       </c>
@@ -3640,8 +4356,11 @@
       <c r="F96" s="1" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G96" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15.75" customHeight="1">
       <c r="A97" t="s">
         <v>105</v>
       </c>
@@ -3660,8 +4379,11 @@
       <c r="F97" s="1" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G97" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15.75" customHeight="1">
       <c r="A98" t="s">
         <v>106</v>
       </c>
@@ -3680,8 +4402,11 @@
       <c r="F98" s="1" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G98" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15.75" customHeight="1">
       <c r="A99" t="s">
         <v>107</v>
       </c>
@@ -3700,8 +4425,11 @@
       <c r="F99" s="1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G99" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15.75" customHeight="1">
       <c r="A100" t="s">
         <v>108</v>
       </c>
@@ -3720,8 +4448,11 @@
       <c r="F100" s="1" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G100" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15.75" customHeight="1">
       <c r="A101" t="s">
         <v>110</v>
       </c>
@@ -3740,8 +4471,11 @@
       <c r="F101" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G101" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15.75" customHeight="1">
       <c r="A102" t="s">
         <v>111</v>
       </c>
@@ -3760,8 +4494,11 @@
       <c r="F102" s="1" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G102" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15.75" customHeight="1">
       <c r="A103" t="s">
         <v>112</v>
       </c>
@@ -3780,8 +4517,11 @@
       <c r="F103" s="1" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G103" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15.75" customHeight="1">
       <c r="A104" t="s">
         <v>113</v>
       </c>
@@ -3800,8 +4540,11 @@
       <c r="F104" s="1" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G104" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15.75" customHeight="1">
       <c r="A105" t="s">
         <v>114</v>
       </c>
@@ -3820,8 +4563,11 @@
       <c r="F105" s="1" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G105" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15.75" customHeight="1">
       <c r="A106" t="s">
         <v>116</v>
       </c>
@@ -3840,8 +4586,11 @@
       <c r="F106" s="1" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G106" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15.75" customHeight="1">
       <c r="A107" t="s">
         <v>117</v>
       </c>
@@ -3860,8 +4609,11 @@
       <c r="F107" s="1" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G107" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15.75" customHeight="1">
       <c r="A108" t="s">
         <v>118</v>
       </c>
@@ -3880,8 +4632,11 @@
       <c r="F108" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G108" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15.75" customHeight="1">
       <c r="A109" t="s">
         <v>119</v>
       </c>
@@ -3900,8 +4655,11 @@
       <c r="F109" s="1" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G109" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15.75" customHeight="1">
       <c r="A110" t="s">
         <v>120</v>
       </c>
@@ -3920,8 +4678,11 @@
       <c r="F110" s="1" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G110" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15.75" customHeight="1">
       <c r="A111" t="s">
         <v>121</v>
       </c>
@@ -3940,8 +4701,11 @@
       <c r="F111" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G111" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15.75" customHeight="1">
       <c r="A112" t="s">
         <v>122</v>
       </c>
@@ -3960,8 +4724,11 @@
       <c r="F112" s="1" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G112" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15.75" customHeight="1">
       <c r="A113" t="s">
         <v>123</v>
       </c>
@@ -3980,8 +4747,11 @@
       <c r="F113" s="1" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G113" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15.75" customHeight="1">
       <c r="A114" t="s">
         <v>125</v>
       </c>
@@ -4000,8 +4770,11 @@
       <c r="F114" s="1" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G114" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15.75" customHeight="1">
       <c r="A115" t="s">
         <v>126</v>
       </c>
@@ -4020,8 +4793,11 @@
       <c r="F115" s="1" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G115" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15.75" customHeight="1">
       <c r="A116" t="s">
         <v>127</v>
       </c>
@@ -4040,8 +4816,11 @@
       <c r="F116" s="1" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G116" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="15.75" customHeight="1">
       <c r="A117" t="s">
         <v>128</v>
       </c>
@@ -4060,8 +4839,11 @@
       <c r="F117" s="1" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G117" s="1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="15.75" customHeight="1">
       <c r="A118" t="s">
         <v>129</v>
       </c>
@@ -4080,8 +4862,11 @@
       <c r="F118" s="1" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G118" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="15.75" customHeight="1">
       <c r="A119" t="s">
         <v>130</v>
       </c>
@@ -4100,8 +4885,11 @@
       <c r="F119" s="1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G119" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="15.75" customHeight="1">
       <c r="A120" t="s">
         <v>131</v>
       </c>
@@ -4120,8 +4908,11 @@
       <c r="F120" s="1" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G120" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15.75" customHeight="1">
       <c r="A121" t="s">
         <v>132</v>
       </c>
@@ -4140,8 +4931,11 @@
       <c r="F121" s="1" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G121" s="1" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15.75" customHeight="1">
       <c r="A122" t="s">
         <v>133</v>
       </c>
@@ -4160,8 +4954,11 @@
       <c r="F122" s="1" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G122" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15.75" customHeight="1">
       <c r="A123" t="s">
         <v>134</v>
       </c>
@@ -4180,8 +4977,11 @@
       <c r="F123" s="1" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G123" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15.75" customHeight="1">
       <c r="A124" t="s">
         <v>135</v>
       </c>
@@ -4200,8 +5000,11 @@
       <c r="F124" s="1" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G124" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="15.75" customHeight="1">
       <c r="A125" t="s">
         <v>136</v>
       </c>
@@ -4220,8 +5023,11 @@
       <c r="F125" s="1" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G125" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="15.75" customHeight="1">
       <c r="A126" t="s">
         <v>137</v>
       </c>
@@ -4240,8 +5046,11 @@
       <c r="F126" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G126" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15.75" customHeight="1">
       <c r="A127" t="s">
         <v>138</v>
       </c>
@@ -4260,8 +5069,11 @@
       <c r="F127" s="1" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G127" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="15.75" customHeight="1">
       <c r="A128" t="s">
         <v>139</v>
       </c>
@@ -4280,8 +5092,11 @@
       <c r="F128" s="1" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G128" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="15.75" customHeight="1">
       <c r="A129" t="s">
         <v>140</v>
       </c>
@@ -4300,8 +5115,11 @@
       <c r="F129" s="1" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G129" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="15.75" customHeight="1">
       <c r="A130" t="s">
         <v>141</v>
       </c>
@@ -4320,8 +5138,11 @@
       <c r="F130" s="1" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G130" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="15.75" customHeight="1">
       <c r="A131" t="s">
         <v>142</v>
       </c>
@@ -4340,8 +5161,11 @@
       <c r="F131" s="1" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G131" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="15.75" customHeight="1">
       <c r="A132" t="s">
         <v>143</v>
       </c>
@@ -4360,8 +5184,11 @@
       <c r="F132" s="1" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G132" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="15.75" customHeight="1">
       <c r="A133" t="s">
         <v>144</v>
       </c>
@@ -4380,8 +5207,11 @@
       <c r="F133" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G133" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="15.75" customHeight="1">
       <c r="A134" t="s">
         <v>145</v>
       </c>
@@ -4400,8 +5230,11 @@
       <c r="F134" s="1" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G134" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="15.75" customHeight="1">
       <c r="A135" t="s">
         <v>147</v>
       </c>
@@ -4420,8 +5253,11 @@
       <c r="F135" s="1" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G135" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="15.75" customHeight="1">
       <c r="A136" t="s">
         <v>148</v>
       </c>
@@ -4440,8 +5276,11 @@
       <c r="F136" s="1" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G136" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="15.75" customHeight="1">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -4460,8 +5299,11 @@
       <c r="F137" s="1" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G137" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="15.75" customHeight="1">
       <c r="A138" t="s">
         <v>150</v>
       </c>
@@ -4480,8 +5322,11 @@
       <c r="F138" s="1" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G138" s="1" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="15.75" customHeight="1">
       <c r="A139" t="s">
         <v>151</v>
       </c>
@@ -4500,8 +5345,11 @@
       <c r="F139" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G139" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="15.75" customHeight="1">
       <c r="A140" t="s">
         <v>152</v>
       </c>
@@ -4520,8 +5368,11 @@
       <c r="F140" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G140" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="15.75" customHeight="1">
       <c r="A141" t="s">
         <v>153</v>
       </c>
@@ -4540,8 +5391,11 @@
       <c r="F141" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G141" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="15.75" customHeight="1">
       <c r="A142" t="s">
         <v>154</v>
       </c>
@@ -4560,8 +5414,11 @@
       <c r="F142" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G142" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="15.75" customHeight="1">
       <c r="A143" t="s">
         <v>155</v>
       </c>
@@ -4579,6 +5436,9 @@
       </c>
       <c r="F143" s="1" t="s">
         <v>447</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>